<commit_message>
Update ingest script to support product reviews, support and add test script to check data retrieval
</commit_message>
<xml_diff>
--- a/data/customer_support.xlsx
+++ b/data/customer_support.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sonnandh/Documents/py/ai-native-commerce-platform/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{72D76922-374B-4B4F-AE17-A27883AAD8EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CE888CC-1EB4-D343-8255-54946E376ABA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{D0C246A5-DF1F-0D4A-87BD-1F6358087DB6}"/>
   </bookViews>
@@ -525,8 +525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D48B646-C22E-CA44-8C73-ED26B1CBC6AE}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView showFormulas="1" tabSelected="1" zoomScale="104" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -547,7 +547,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="365" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="96" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -558,7 +558,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="350" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="96" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -569,7 +569,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="256" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -580,7 +580,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="365" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="112" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -591,7 +591,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="240" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -602,7 +602,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="240" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="80" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -613,7 +613,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="288" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="80" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
@@ -624,7 +624,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="380" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="112" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
@@ -635,7 +635,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="272" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="80" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
@@ -646,7 +646,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="272" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="80" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>

</xml_diff>